<commit_message>
Fix DTC DrankkaartType en gebruikerController, RoleController
</commit_message>
<xml_diff>
--- a/Startspeler/planning.xlsx
+++ b/Startspeler/planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Startspeler\Startspeler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE773230-2361-4A4C-BF9D-2BAC23220B55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24F7F7B-4D0C-4A4F-B198-CD5158091FCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5BD469D0-082D-4F4A-A9D5-19CCB8849940}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5BD469D0-082D-4F4A-A9D5-19CCB8849940}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
   <si>
     <t>Item</t>
   </si>
@@ -193,6 +193,21 @@
   </si>
   <si>
     <t>Nice to have</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Handleiding </t>
+  </si>
+  <si>
+    <t>Privacy pagina</t>
+  </si>
+  <si>
+    <t>nice to have</t>
+  </si>
+  <si>
+    <t>inleveren project</t>
+  </si>
+  <si>
+    <t>presentatie</t>
   </si>
 </sst>
 </file>
@@ -247,7 +262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -361,11 +376,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -433,15 +472,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -467,11 +497,23 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -787,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D68F08FA-29DA-4B46-BA48-133A986F2823}">
-  <dimension ref="D2:G53"/>
+  <dimension ref="D2:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1046,13 +1088,13 @@
       </c>
     </row>
     <row r="25" spans="4:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="31">
+      <c r="E25" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="28">
         <v>44327</v>
       </c>
     </row>
@@ -1208,15 +1250,15 @@
       <c r="D40" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E40" s="26" t="s">
+      <c r="E40" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="27">
+      <c r="F40" s="24">
         <v>44333</v>
       </c>
     </row>
     <row r="41" spans="4:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D41" s="28" t="s">
+      <c r="D41" s="25" t="s">
         <v>48</v>
       </c>
       <c r="E41" s="21" t="s">
@@ -1298,31 +1340,31 @@
       </c>
     </row>
     <row r="49" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="E49" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49" s="10">
         <v>44334</v>
       </c>
     </row>
     <row r="50" spans="4:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D50" s="35" t="s">
+      <c r="D50" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E50" s="33" t="s">
+      <c r="E50" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="F50" s="36">
+      <c r="F50" s="33">
         <v>44334</v>
       </c>
     </row>
     <row r="51" spans="4:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D51" s="32"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="34"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="31"/>
     </row>
     <row r="52" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D52" s="4" t="s">
@@ -1336,14 +1378,47 @@
       </c>
     </row>
     <row r="53" spans="4:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D53" s="23" t="s">
+      <c r="D53" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E53" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="F53" s="25">
+      <c r="E53" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="33">
         <v>44341</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D54" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E54" s="35"/>
+      <c r="F54" s="36">
+        <v>44358</v>
+      </c>
+    </row>
+    <row r="55" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>54</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>56</v>
+      </c>
+      <c r="F57" s="37">
+        <v>44353</v>
+      </c>
+    </row>
+    <row r="60" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>57</v>
+      </c>
+      <c r="F60" s="37">
+        <v>44363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update planning to reflect everything is done as planned
</commit_message>
<xml_diff>
--- a/Startspeler/planning.xlsx
+++ b/Startspeler/planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sterc\Documents\Thomas More\Repositories\Startspeler\Startspeler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Startspeler\Startspeler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA94933-198A-4C84-B43D-9A7C25392905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A73A64C-C3A6-4DAE-9787-CF650AAFC487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="360" windowWidth="28770" windowHeight="15570" xr2:uid="{5BD469D0-082D-4F4A-A9D5-19CCB8849940}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5BD469D0-082D-4F4A-A9D5-19CCB8849940}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="58">
   <si>
     <t>Item</t>
   </si>
@@ -374,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -430,19 +430,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -467,14 +460,10 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -792,20 +781,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D68F08FA-29DA-4B46-BA48-133A986F2823}">
   <dimension ref="D2:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="83.140625" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="83.109375" customWidth="1"/>
+    <col min="5" max="5" width="42.5546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="55" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D3" s="10" t="s">
         <v>0</v>
       </c>
@@ -817,7 +806,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
@@ -828,7 +817,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D5" s="7" t="s">
         <v>2</v>
       </c>
@@ -839,7 +828,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D6" s="7" t="s">
         <v>3</v>
       </c>
@@ -850,7 +839,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
@@ -861,7 +850,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D8" s="7" t="s">
         <v>6</v>
       </c>
@@ -872,7 +861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D9" s="7" t="s">
         <v>7</v>
       </c>
@@ -883,7 +872,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D10" s="7" t="s">
         <v>8</v>
       </c>
@@ -894,7 +883,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D11" s="7" t="s">
         <v>5</v>
       </c>
@@ -905,7 +894,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D12" s="7" t="s">
         <v>6</v>
       </c>
@@ -916,7 +905,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="7" t="s">
         <v>7</v>
       </c>
@@ -927,7 +916,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D14" s="7" t="s">
         <v>8</v>
       </c>
@@ -938,7 +927,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D15" s="3" t="s">
         <v>16</v>
       </c>
@@ -949,7 +938,7 @@
         <v>44313</v>
       </c>
     </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D16" s="3" t="s">
         <v>17</v>
       </c>
@@ -960,7 +949,7 @@
         <v>44313</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D17" s="3" t="s">
         <v>32</v>
       </c>
@@ -971,7 +960,7 @@
         <v>44320</v>
       </c>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D18" s="3" t="s">
         <v>33</v>
       </c>
@@ -982,7 +971,7 @@
         <v>44327</v>
       </c>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D19" s="3" t="s">
         <v>44</v>
       </c>
@@ -993,7 +982,7 @@
         <v>44320</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D20" s="3" t="s">
         <v>29</v>
       </c>
@@ -1004,7 +993,7 @@
         <v>44313</v>
       </c>
     </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D21" s="3" t="s">
         <v>30</v>
       </c>
@@ -1015,7 +1004,7 @@
         <v>44327</v>
       </c>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D22" s="3" t="s">
         <v>45</v>
       </c>
@@ -1026,7 +1015,7 @@
         <v>44320</v>
       </c>
     </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D23" s="3" t="s">
         <v>34</v>
       </c>
@@ -1037,7 +1026,7 @@
         <v>44327</v>
       </c>
     </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D24" s="3" t="s">
         <v>31</v>
       </c>
@@ -1048,23 +1037,23 @@
         <v>44327</v>
       </c>
     </row>
-    <row r="25" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="24" t="s">
+    <row r="25" spans="4:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="26">
+      <c r="E25" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="23">
         <v>44327</v>
       </c>
     </row>
-    <row r="26" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D26" s="14"/>
       <c r="E26" s="15"/>
       <c r="F26" s="16"/>
     </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D27" s="4" t="s">
         <v>25</v>
       </c>
@@ -1075,7 +1064,7 @@
         <v>44313</v>
       </c>
     </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D28" s="3" t="s">
         <v>46</v>
       </c>
@@ -1086,7 +1075,7 @@
         <v>44313</v>
       </c>
     </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D29" s="3" t="s">
         <v>26</v>
       </c>
@@ -1097,7 +1086,7 @@
         <v>44313</v>
       </c>
     </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D30" s="3" t="s">
         <v>49</v>
       </c>
@@ -1108,7 +1097,7 @@
         <v>44320</v>
       </c>
     </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D31" s="3" t="s">
         <v>28</v>
       </c>
@@ -1119,7 +1108,7 @@
         <v>44320</v>
       </c>
     </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D32" s="3" t="s">
         <v>35</v>
       </c>
@@ -1130,7 +1119,7 @@
         <v>44313</v>
       </c>
     </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D33" s="3" t="s">
         <v>36</v>
       </c>
@@ -1141,7 +1130,7 @@
         <v>44313</v>
       </c>
     </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D34" s="3" t="s">
         <v>50</v>
       </c>
@@ -1152,7 +1141,7 @@
         <v>44313</v>
       </c>
     </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D35" s="3" t="s">
         <v>38</v>
       </c>
@@ -1163,7 +1152,7 @@
         <v>44313</v>
       </c>
     </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D36" s="3" t="s">
         <v>27</v>
       </c>
@@ -1174,7 +1163,7 @@
         <v>44327</v>
       </c>
     </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D37" s="3" t="s">
         <v>42</v>
       </c>
@@ -1185,7 +1174,7 @@
         <v>44341</v>
       </c>
     </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D38" s="3" t="s">
         <v>37</v>
       </c>
@@ -1196,7 +1185,7 @@
         <v>44327</v>
       </c>
     </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D39" s="3" t="s">
         <v>41</v>
       </c>
@@ -1207,34 +1196,34 @@
         <v>44341</v>
       </c>
     </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D40" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E40" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F40" s="22">
+      <c r="E40" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="20">
         <v>44333</v>
       </c>
     </row>
-    <row r="41" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="23" t="s">
+    <row r="41" spans="4:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D41" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E41" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41" s="20" t="s">
+      <c r="E41" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="23" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D42" s="14"/>
       <c r="E42" s="15"/>
       <c r="F42" s="16"/>
     </row>
-    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D43" s="4" t="s">
         <v>19</v>
       </c>
@@ -1245,7 +1234,7 @@
         <v>44327</v>
       </c>
     </row>
-    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D44" s="3" t="s">
         <v>20</v>
       </c>
@@ -1256,7 +1245,7 @@
         <v>44327</v>
       </c>
     </row>
-    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D45" s="3" t="s">
         <v>21</v>
       </c>
@@ -1267,7 +1256,7 @@
         <v>44327</v>
       </c>
     </row>
-    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D46" s="3" t="s">
         <v>22</v>
       </c>
@@ -1278,7 +1267,7 @@
         <v>44327</v>
       </c>
     </row>
-    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D47" s="3" t="s">
         <v>23</v>
       </c>
@@ -1289,7 +1278,7 @@
         <v>44327</v>
       </c>
     </row>
-    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D48" s="3" t="s">
         <v>24</v>
       </c>
@@ -1300,7 +1289,7 @@
         <v>44327</v>
       </c>
     </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D49" s="7" t="s">
         <v>39</v>
       </c>
@@ -1311,34 +1300,34 @@
         <v>44334</v>
       </c>
     </row>
-    <row r="50" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D50" s="24" t="s">
+    <row r="50" spans="4:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D50" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E50" s="27" t="s">
+      <c r="E50" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="F50" s="28">
+      <c r="F50" s="25">
         <v>44334</v>
       </c>
     </row>
-    <row r="51" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="30"/>
+    <row r="51" spans="4:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D51" s="27"/>
       <c r="E51" s="13"/>
-      <c r="F51" s="31"/>
-    </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D52" s="32" t="s">
+      <c r="F51" s="28"/>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D52" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E52" s="33" t="s">
+      <c r="E52" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="F52" s="34">
+      <c r="F52" s="9">
         <v>44341</v>
       </c>
     </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D53" s="7" t="s">
         <v>4</v>
       </c>
@@ -1349,38 +1338,41 @@
         <v>44341</v>
       </c>
     </row>
-    <row r="54" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="24" t="s">
+    <row r="54" spans="4:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D54" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E54" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F54" s="26">
+      <c r="E54" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="23">
         <v>44358</v>
       </c>
     </row>
-    <row r="55" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D55" t="s">
+    <row r="55" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D55" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="E55" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
         <v>56</v>
       </c>
-      <c r="F57" s="29">
+      <c r="F57" s="26">
         <v>44353</v>
       </c>
     </row>
-    <row r="60" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D60" t="s">
         <v>57</v>
       </c>
-      <c r="F60" s="29">
+      <c r="F60" s="26">
         <v>44363</v>
       </c>
     </row>

</xml_diff>